<commit_message>
move coords column + rename test transfer sample file
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Sample_transfer_v4_6_0.xlsx
+++ b/backend/fms_core/static/submission_templates/Sample_transfer_v4_6_0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jmarcelino/Desktop/freezeman/backend/fms_core/static/submission_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71F20DCF-429A-BA43-9032-4FE3D398DA31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D78A9468-2F54-1D46-A509-35ACF35AE69A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="700" windowWidth="27040" windowHeight="16860" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="960" yWindow="8080" windowWidth="27040" windowHeight="11560" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SampleTransfer" sheetId="1" r:id="rId1"/>
@@ -74,9 +74,6 @@
     </r>
   </si>
   <si>
-    <t>Version : 4.4.0</t>
-  </si>
-  <si>
     <t>*</t>
   </si>
   <si>
@@ -1383,6 +1380,9 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>Version : 4.6.0</t>
   </si>
 </sst>
 </file>
@@ -1842,7 +1842,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1912,8 +1912,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2299,8 +2301,8 @@
   <dimension ref="A1:AD708"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A84" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
+      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -2331,11 +2333,11 @@
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>2</v>
+      <c r="B2" s="39" t="s">
+        <v>438</v>
       </c>
       <c r="D2" s="40" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E2" s="14"/>
     </row>
@@ -2348,22 +2350,22 @@
     </row>
     <row r="4" spans="1:30" ht="15" x14ac:dyDescent="0.2">
       <c r="B4" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P4" s="4"/>
       <c r="T4" s="4"/>
@@ -2372,60 +2374,60 @@
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="C5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="D5" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="E5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="F5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="G5" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="H5" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="I5" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="I5" s="11" t="s">
+      <c r="J5" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="J5" s="12" t="s">
+      <c r="K5" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="K5" s="12" t="s">
+      <c r="L5" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="L5" s="12" t="s">
+      <c r="M5" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="M5" s="7" t="s">
+      <c r="N5" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="N5" s="6" t="s">
+      <c r="O5" s="13" t="s">
         <v>17</v>
-      </c>
-      <c r="O5" s="13" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:30" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="14"/>
       <c r="B6" s="15"/>
       <c r="C6" s="15"/>
-      <c r="D6" s="41" t="str">
+      <c r="D6" s="41"/>
+      <c r="E6" s="43" t="str">
         <f>IF(AND(E$2="Yes",NOT(ISBLANK($C6))),C6,"")</f>
         <v/>
       </c>
-      <c r="E6" s="16"/>
       <c r="F6" s="16"/>
       <c r="G6" s="17"/>
       <c r="H6" s="18"/>
@@ -2441,11 +2443,11 @@
       <c r="A7" s="14"/>
       <c r="B7" s="15"/>
       <c r="C7" s="15"/>
-      <c r="D7" s="41" t="str">
-        <f>IF(AND(E$2="Yes",NOT(ISBLANK($C7))),C7,"")</f>
-        <v/>
-      </c>
-      <c r="E7" s="16"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="43" t="str">
+        <f t="shared" ref="E7:E70" si="0">IF(AND(E$2="Yes",NOT(ISBLANK($C7))),C7,"")</f>
+        <v/>
+      </c>
       <c r="F7" s="16"/>
       <c r="G7" s="17"/>
       <c r="H7" s="18"/>
@@ -2461,11 +2463,11 @@
       <c r="A8" s="14"/>
       <c r="B8" s="15"/>
       <c r="C8" s="15"/>
-      <c r="D8" s="41" t="str">
-        <f t="shared" ref="D8:D71" si="0">IF(AND(E$2="Yes",NOT(ISBLANK($C8))),C8,"")</f>
-        <v/>
-      </c>
-      <c r="E8" s="16"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="43" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="F8" s="16"/>
       <c r="G8" s="17"/>
       <c r="H8" s="18"/>
@@ -2481,11 +2483,11 @@
       <c r="A9" s="14"/>
       <c r="B9" s="15"/>
       <c r="C9" s="15"/>
-      <c r="D9" s="41" t="str">
+      <c r="D9" s="41"/>
+      <c r="E9" s="43" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="E9" s="16"/>
       <c r="F9" s="16"/>
       <c r="G9" s="17"/>
       <c r="H9" s="18"/>
@@ -2501,11 +2503,11 @@
       <c r="A10" s="14"/>
       <c r="B10" s="15"/>
       <c r="C10" s="15"/>
-      <c r="D10" s="41" t="str">
+      <c r="D10" s="41"/>
+      <c r="E10" s="43" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="E10" s="16"/>
       <c r="F10" s="16"/>
       <c r="G10" s="17"/>
       <c r="H10" s="18"/>
@@ -2521,11 +2523,11 @@
       <c r="A11" s="14"/>
       <c r="B11" s="15"/>
       <c r="C11" s="15"/>
-      <c r="D11" s="41" t="str">
+      <c r="D11" s="41"/>
+      <c r="E11" s="43" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="E11" s="16"/>
       <c r="F11" s="16"/>
       <c r="G11" s="17"/>
       <c r="H11" s="18"/>
@@ -2541,11 +2543,11 @@
       <c r="A12" s="14"/>
       <c r="B12" s="15"/>
       <c r="C12" s="15"/>
-      <c r="D12" s="41" t="str">
+      <c r="D12" s="41"/>
+      <c r="E12" s="43" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="E12" s="16"/>
       <c r="F12" s="16"/>
       <c r="G12" s="17"/>
       <c r="H12" s="18"/>
@@ -2561,11 +2563,11 @@
       <c r="A13" s="14"/>
       <c r="B13" s="15"/>
       <c r="C13" s="15"/>
-      <c r="D13" s="41" t="str">
+      <c r="D13" s="41"/>
+      <c r="E13" s="43" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="E13" s="16"/>
       <c r="F13" s="16"/>
       <c r="G13" s="17"/>
       <c r="H13" s="18"/>
@@ -2581,11 +2583,11 @@
       <c r="A14" s="14"/>
       <c r="B14" s="15"/>
       <c r="C14" s="15"/>
-      <c r="D14" s="41" t="str">
+      <c r="D14" s="41"/>
+      <c r="E14" s="43" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="E14" s="16"/>
       <c r="F14" s="16"/>
       <c r="G14" s="17"/>
       <c r="H14" s="18"/>
@@ -2601,11 +2603,11 @@
       <c r="A15" s="14"/>
       <c r="B15" s="15"/>
       <c r="C15" s="15"/>
-      <c r="D15" s="41" t="str">
+      <c r="D15" s="41"/>
+      <c r="E15" s="43" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="E15" s="16"/>
       <c r="F15" s="16"/>
       <c r="G15" s="17"/>
       <c r="H15" s="18"/>
@@ -2621,11 +2623,11 @@
       <c r="A16" s="14"/>
       <c r="B16" s="15"/>
       <c r="C16" s="15"/>
-      <c r="D16" s="41" t="str">
+      <c r="D16" s="41"/>
+      <c r="E16" s="43" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="E16" s="16"/>
       <c r="F16" s="16"/>
       <c r="G16" s="17"/>
       <c r="H16" s="18"/>
@@ -2641,11 +2643,11 @@
       <c r="A17" s="14"/>
       <c r="B17" s="15"/>
       <c r="C17" s="15"/>
-      <c r="D17" s="41" t="str">
+      <c r="D17" s="41"/>
+      <c r="E17" s="43" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="E17" s="16"/>
       <c r="F17" s="16"/>
       <c r="G17" s="17"/>
       <c r="H17" s="18"/>
@@ -2661,11 +2663,11 @@
       <c r="A18" s="14"/>
       <c r="B18" s="15"/>
       <c r="C18" s="15"/>
-      <c r="D18" s="41" t="str">
+      <c r="D18" s="41"/>
+      <c r="E18" s="43" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="E18" s="16"/>
       <c r="F18" s="16"/>
       <c r="G18" s="17"/>
       <c r="H18" s="18"/>
@@ -2681,11 +2683,11 @@
       <c r="A19" s="14"/>
       <c r="B19" s="15"/>
       <c r="C19" s="15"/>
-      <c r="D19" s="41" t="str">
+      <c r="D19" s="41"/>
+      <c r="E19" s="43" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="E19" s="16"/>
       <c r="F19" s="16"/>
       <c r="G19" s="17"/>
       <c r="H19" s="18"/>
@@ -2701,11 +2703,11 @@
       <c r="A20" s="14"/>
       <c r="B20" s="15"/>
       <c r="C20" s="15"/>
-      <c r="D20" s="41" t="str">
+      <c r="D20" s="41"/>
+      <c r="E20" s="43" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="E20" s="16"/>
       <c r="F20" s="16"/>
       <c r="G20" s="17"/>
       <c r="H20" s="18"/>
@@ -2721,11 +2723,11 @@
       <c r="A21" s="14"/>
       <c r="B21" s="15"/>
       <c r="C21" s="15"/>
-      <c r="D21" s="41" t="str">
+      <c r="D21" s="41"/>
+      <c r="E21" s="43" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="E21" s="16"/>
       <c r="F21" s="16"/>
       <c r="G21" s="17"/>
       <c r="H21" s="18"/>
@@ -2741,11 +2743,11 @@
       <c r="A22" s="14"/>
       <c r="B22" s="15"/>
       <c r="C22" s="15"/>
-      <c r="D22" s="41" t="str">
+      <c r="D22" s="41"/>
+      <c r="E22" s="43" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="E22" s="16"/>
       <c r="F22" s="16"/>
       <c r="G22" s="17"/>
       <c r="H22" s="18"/>
@@ -2761,11 +2763,11 @@
       <c r="A23" s="14"/>
       <c r="B23" s="15"/>
       <c r="C23" s="15"/>
-      <c r="D23" s="41" t="str">
+      <c r="D23" s="41"/>
+      <c r="E23" s="43" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="E23" s="16"/>
       <c r="F23" s="16"/>
       <c r="G23" s="17"/>
       <c r="H23" s="18"/>
@@ -2781,11 +2783,11 @@
       <c r="A24" s="14"/>
       <c r="B24" s="15"/>
       <c r="C24" s="15"/>
-      <c r="D24" s="41" t="str">
+      <c r="D24" s="41"/>
+      <c r="E24" s="43" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="E24" s="16"/>
       <c r="F24" s="16"/>
       <c r="G24" s="17"/>
       <c r="H24" s="18"/>
@@ -2801,11 +2803,11 @@
       <c r="A25" s="14"/>
       <c r="B25" s="15"/>
       <c r="C25" s="15"/>
-      <c r="D25" s="41" t="str">
+      <c r="D25" s="41"/>
+      <c r="E25" s="43" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="E25" s="16"/>
       <c r="F25" s="16"/>
       <c r="G25" s="17"/>
       <c r="H25" s="18"/>
@@ -2821,11 +2823,11 @@
       <c r="A26" s="14"/>
       <c r="B26" s="15"/>
       <c r="C26" s="15"/>
-      <c r="D26" s="41" t="str">
+      <c r="D26" s="41"/>
+      <c r="E26" s="43" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="E26" s="16"/>
       <c r="F26" s="16"/>
       <c r="G26" s="17"/>
       <c r="H26" s="18"/>
@@ -2841,11 +2843,11 @@
       <c r="A27" s="14"/>
       <c r="B27" s="15"/>
       <c r="C27" s="15"/>
-      <c r="D27" s="41" t="str">
+      <c r="D27" s="41"/>
+      <c r="E27" s="43" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="E27" s="16"/>
       <c r="F27" s="16"/>
       <c r="G27" s="17"/>
       <c r="H27" s="18"/>
@@ -2861,11 +2863,11 @@
       <c r="A28" s="14"/>
       <c r="B28" s="15"/>
       <c r="C28" s="15"/>
-      <c r="D28" s="41" t="str">
+      <c r="D28" s="41"/>
+      <c r="E28" s="43" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="E28" s="16"/>
       <c r="F28" s="16"/>
       <c r="G28" s="17"/>
       <c r="H28" s="18"/>
@@ -2881,11 +2883,11 @@
       <c r="A29" s="14"/>
       <c r="B29" s="15"/>
       <c r="C29" s="15"/>
-      <c r="D29" s="41" t="str">
+      <c r="D29" s="41"/>
+      <c r="E29" s="43" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="E29" s="16"/>
       <c r="F29" s="16"/>
       <c r="G29" s="17"/>
       <c r="H29" s="18"/>
@@ -2901,11 +2903,11 @@
       <c r="A30" s="14"/>
       <c r="B30" s="15"/>
       <c r="C30" s="15"/>
-      <c r="D30" s="41" t="str">
+      <c r="D30" s="41"/>
+      <c r="E30" s="43" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="E30" s="16"/>
       <c r="F30" s="16"/>
       <c r="G30" s="17"/>
       <c r="H30" s="18"/>
@@ -2921,11 +2923,11 @@
       <c r="A31" s="14"/>
       <c r="B31" s="15"/>
       <c r="C31" s="15"/>
-      <c r="D31" s="41" t="str">
+      <c r="D31" s="41"/>
+      <c r="E31" s="43" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="E31" s="16"/>
       <c r="F31" s="16"/>
       <c r="G31" s="17"/>
       <c r="H31" s="18"/>
@@ -2941,11 +2943,11 @@
       <c r="A32" s="14"/>
       <c r="B32" s="15"/>
       <c r="C32" s="15"/>
-      <c r="D32" s="41" t="str">
+      <c r="D32" s="41"/>
+      <c r="E32" s="43" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="E32" s="16"/>
       <c r="F32" s="16"/>
       <c r="G32" s="17"/>
       <c r="H32" s="18"/>
@@ -2961,11 +2963,11 @@
       <c r="A33" s="14"/>
       <c r="B33" s="15"/>
       <c r="C33" s="15"/>
-      <c r="D33" s="41" t="str">
+      <c r="D33" s="41"/>
+      <c r="E33" s="43" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="E33" s="16"/>
       <c r="F33" s="16"/>
       <c r="G33" s="17"/>
       <c r="H33" s="18"/>
@@ -2981,11 +2983,11 @@
       <c r="A34" s="14"/>
       <c r="B34" s="15"/>
       <c r="C34" s="15"/>
-      <c r="D34" s="41" t="str">
+      <c r="D34" s="41"/>
+      <c r="E34" s="43" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="E34" s="16"/>
       <c r="F34" s="16"/>
       <c r="G34" s="17"/>
       <c r="H34" s="18"/>
@@ -3001,11 +3003,11 @@
       <c r="A35" s="14"/>
       <c r="B35" s="15"/>
       <c r="C35" s="15"/>
-      <c r="D35" s="41" t="str">
+      <c r="D35" s="41"/>
+      <c r="E35" s="43" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="E35" s="16"/>
       <c r="F35" s="16"/>
       <c r="G35" s="17"/>
       <c r="H35" s="18"/>
@@ -3021,11 +3023,11 @@
       <c r="A36" s="14"/>
       <c r="B36" s="15"/>
       <c r="C36" s="15"/>
-      <c r="D36" s="41" t="str">
+      <c r="D36" s="41"/>
+      <c r="E36" s="43" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="E36" s="16"/>
       <c r="F36" s="16"/>
       <c r="G36" s="17"/>
       <c r="H36" s="18"/>
@@ -3041,11 +3043,11 @@
       <c r="A37" s="14"/>
       <c r="B37" s="15"/>
       <c r="C37" s="15"/>
-      <c r="D37" s="41" t="str">
+      <c r="D37" s="41"/>
+      <c r="E37" s="43" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="E37" s="16"/>
       <c r="F37" s="16"/>
       <c r="G37" s="17"/>
       <c r="H37" s="18"/>
@@ -3061,11 +3063,11 @@
       <c r="A38" s="14"/>
       <c r="B38" s="15"/>
       <c r="C38" s="15"/>
-      <c r="D38" s="41" t="str">
+      <c r="D38" s="41"/>
+      <c r="E38" s="43" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="E38" s="16"/>
       <c r="F38" s="16"/>
       <c r="G38" s="17"/>
       <c r="H38" s="18"/>
@@ -3081,11 +3083,11 @@
       <c r="A39" s="14"/>
       <c r="B39" s="15"/>
       <c r="C39" s="15"/>
-      <c r="D39" s="41" t="str">
+      <c r="D39" s="41"/>
+      <c r="E39" s="43" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="E39" s="16"/>
       <c r="F39" s="16"/>
       <c r="G39" s="17"/>
       <c r="H39" s="18"/>
@@ -3101,11 +3103,11 @@
       <c r="A40" s="14"/>
       <c r="B40" s="15"/>
       <c r="C40" s="15"/>
-      <c r="D40" s="41" t="str">
+      <c r="D40" s="41"/>
+      <c r="E40" s="43" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="E40" s="16"/>
       <c r="F40" s="16"/>
       <c r="G40" s="17"/>
       <c r="H40" s="18"/>
@@ -3121,11 +3123,11 @@
       <c r="A41" s="14"/>
       <c r="B41" s="15"/>
       <c r="C41" s="15"/>
-      <c r="D41" s="41" t="str">
+      <c r="D41" s="41"/>
+      <c r="E41" s="43" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="E41" s="16"/>
       <c r="F41" s="16"/>
       <c r="G41" s="17"/>
       <c r="H41" s="18"/>
@@ -3141,11 +3143,11 @@
       <c r="A42" s="14"/>
       <c r="B42" s="15"/>
       <c r="C42" s="15"/>
-      <c r="D42" s="41" t="str">
+      <c r="D42" s="41"/>
+      <c r="E42" s="43" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="E42" s="16"/>
       <c r="F42" s="16"/>
       <c r="G42" s="17"/>
       <c r="H42" s="18"/>
@@ -3161,11 +3163,11 @@
       <c r="A43" s="14"/>
       <c r="B43" s="15"/>
       <c r="C43" s="15"/>
-      <c r="D43" s="41" t="str">
+      <c r="D43" s="41"/>
+      <c r="E43" s="43" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="E43" s="16"/>
       <c r="F43" s="16"/>
       <c r="G43" s="17"/>
       <c r="H43" s="18"/>
@@ -3181,11 +3183,11 @@
       <c r="A44" s="14"/>
       <c r="B44" s="15"/>
       <c r="C44" s="15"/>
-      <c r="D44" s="41" t="str">
+      <c r="D44" s="41"/>
+      <c r="E44" s="43" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="E44" s="16"/>
       <c r="F44" s="16"/>
       <c r="G44" s="17"/>
       <c r="H44" s="18"/>
@@ -3201,11 +3203,11 @@
       <c r="A45" s="14"/>
       <c r="B45" s="15"/>
       <c r="C45" s="15"/>
-      <c r="D45" s="41" t="str">
+      <c r="D45" s="41"/>
+      <c r="E45" s="43" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="E45" s="16"/>
       <c r="F45" s="16"/>
       <c r="G45" s="17"/>
       <c r="H45" s="18"/>
@@ -3221,11 +3223,11 @@
       <c r="A46" s="14"/>
       <c r="B46" s="15"/>
       <c r="C46" s="15"/>
-      <c r="D46" s="41" t="str">
+      <c r="D46" s="41"/>
+      <c r="E46" s="43" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="E46" s="16"/>
       <c r="F46" s="16"/>
       <c r="G46" s="17"/>
       <c r="H46" s="18"/>
@@ -3241,11 +3243,11 @@
       <c r="A47" s="14"/>
       <c r="B47" s="15"/>
       <c r="C47" s="15"/>
-      <c r="D47" s="41" t="str">
+      <c r="D47" s="41"/>
+      <c r="E47" s="43" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="E47" s="16"/>
       <c r="F47" s="16"/>
       <c r="G47" s="17"/>
       <c r="H47" s="18"/>
@@ -3261,11 +3263,11 @@
       <c r="A48" s="14"/>
       <c r="B48" s="15"/>
       <c r="C48" s="15"/>
-      <c r="D48" s="41" t="str">
+      <c r="D48" s="41"/>
+      <c r="E48" s="43" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="E48" s="16"/>
       <c r="F48" s="16"/>
       <c r="G48" s="17"/>
       <c r="H48" s="18"/>
@@ -3281,11 +3283,11 @@
       <c r="A49" s="14"/>
       <c r="B49" s="15"/>
       <c r="C49" s="15"/>
-      <c r="D49" s="41" t="str">
+      <c r="D49" s="41"/>
+      <c r="E49" s="43" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="E49" s="16"/>
       <c r="F49" s="16"/>
       <c r="G49" s="17"/>
       <c r="H49" s="18"/>
@@ -3301,11 +3303,11 @@
       <c r="A50" s="14"/>
       <c r="B50" s="15"/>
       <c r="C50" s="15"/>
-      <c r="D50" s="41" t="str">
+      <c r="D50" s="41"/>
+      <c r="E50" s="43" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="E50" s="16"/>
       <c r="F50" s="16"/>
       <c r="G50" s="17"/>
       <c r="H50" s="18"/>
@@ -3321,11 +3323,11 @@
       <c r="A51" s="14"/>
       <c r="B51" s="15"/>
       <c r="C51" s="15"/>
-      <c r="D51" s="41" t="str">
+      <c r="D51" s="41"/>
+      <c r="E51" s="43" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="E51" s="16"/>
       <c r="F51" s="16"/>
       <c r="G51" s="17"/>
       <c r="H51" s="18"/>
@@ -3341,11 +3343,11 @@
       <c r="A52" s="14"/>
       <c r="B52" s="15"/>
       <c r="C52" s="15"/>
-      <c r="D52" s="41" t="str">
+      <c r="D52" s="41"/>
+      <c r="E52" s="43" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="E52" s="16"/>
       <c r="F52" s="16"/>
       <c r="G52" s="17"/>
       <c r="H52" s="18"/>
@@ -3361,11 +3363,11 @@
       <c r="A53" s="14"/>
       <c r="B53" s="15"/>
       <c r="C53" s="15"/>
-      <c r="D53" s="41" t="str">
+      <c r="D53" s="41"/>
+      <c r="E53" s="43" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="E53" s="16"/>
       <c r="F53" s="16"/>
       <c r="G53" s="17"/>
       <c r="H53" s="18"/>
@@ -3381,11 +3383,11 @@
       <c r="A54" s="14"/>
       <c r="B54" s="15"/>
       <c r="C54" s="15"/>
-      <c r="D54" s="41" t="str">
+      <c r="D54" s="41"/>
+      <c r="E54" s="43" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="E54" s="16"/>
       <c r="F54" s="16"/>
       <c r="G54" s="17"/>
       <c r="H54" s="18"/>
@@ -3401,11 +3403,11 @@
       <c r="A55" s="14"/>
       <c r="B55" s="15"/>
       <c r="C55" s="15"/>
-      <c r="D55" s="41" t="str">
+      <c r="D55" s="41"/>
+      <c r="E55" s="43" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="E55" s="16"/>
       <c r="F55" s="16"/>
       <c r="G55" s="17"/>
       <c r="H55" s="18"/>
@@ -3421,11 +3423,11 @@
       <c r="A56" s="14"/>
       <c r="B56" s="15"/>
       <c r="C56" s="15"/>
-      <c r="D56" s="41" t="str">
+      <c r="D56" s="41"/>
+      <c r="E56" s="43" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="E56" s="16"/>
       <c r="F56" s="16"/>
       <c r="G56" s="17"/>
       <c r="H56" s="18"/>
@@ -3441,11 +3443,11 @@
       <c r="A57" s="14"/>
       <c r="B57" s="15"/>
       <c r="C57" s="15"/>
-      <c r="D57" s="41" t="str">
+      <c r="D57" s="41"/>
+      <c r="E57" s="43" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="E57" s="16"/>
       <c r="F57" s="16"/>
       <c r="G57" s="17"/>
       <c r="H57" s="18"/>
@@ -3461,11 +3463,11 @@
       <c r="A58" s="14"/>
       <c r="B58" s="15"/>
       <c r="C58" s="15"/>
-      <c r="D58" s="41" t="str">
+      <c r="D58" s="41"/>
+      <c r="E58" s="43" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="E58" s="16"/>
       <c r="F58" s="16"/>
       <c r="G58" s="17"/>
       <c r="H58" s="18"/>
@@ -3481,11 +3483,11 @@
       <c r="A59" s="14"/>
       <c r="B59" s="15"/>
       <c r="C59" s="15"/>
-      <c r="D59" s="41" t="str">
+      <c r="D59" s="41"/>
+      <c r="E59" s="43" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="E59" s="16"/>
       <c r="F59" s="16"/>
       <c r="G59" s="17"/>
       <c r="H59" s="18"/>
@@ -3501,11 +3503,11 @@
       <c r="A60" s="14"/>
       <c r="B60" s="15"/>
       <c r="C60" s="15"/>
-      <c r="D60" s="41" t="str">
+      <c r="D60" s="41"/>
+      <c r="E60" s="43" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="E60" s="16"/>
       <c r="F60" s="16"/>
       <c r="G60" s="17"/>
       <c r="H60" s="18"/>
@@ -3521,11 +3523,11 @@
       <c r="A61" s="14"/>
       <c r="B61" s="15"/>
       <c r="C61" s="15"/>
-      <c r="D61" s="41" t="str">
+      <c r="D61" s="41"/>
+      <c r="E61" s="43" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="E61" s="16"/>
       <c r="F61" s="16"/>
       <c r="G61" s="17"/>
       <c r="H61" s="18"/>
@@ -3541,11 +3543,11 @@
       <c r="A62" s="14"/>
       <c r="B62" s="15"/>
       <c r="C62" s="15"/>
-      <c r="D62" s="41" t="str">
+      <c r="D62" s="41"/>
+      <c r="E62" s="43" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="E62" s="16"/>
       <c r="F62" s="16"/>
       <c r="G62" s="17"/>
       <c r="H62" s="18"/>
@@ -3561,11 +3563,11 @@
       <c r="A63" s="14"/>
       <c r="B63" s="15"/>
       <c r="C63" s="15"/>
-      <c r="D63" s="41" t="str">
+      <c r="D63" s="41"/>
+      <c r="E63" s="43" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="E63" s="16"/>
       <c r="F63" s="16"/>
       <c r="G63" s="17"/>
       <c r="H63" s="18"/>
@@ -3581,11 +3583,11 @@
       <c r="A64" s="14"/>
       <c r="B64" s="15"/>
       <c r="C64" s="15"/>
-      <c r="D64" s="41" t="str">
+      <c r="D64" s="41"/>
+      <c r="E64" s="43" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="E64" s="16"/>
       <c r="F64" s="16"/>
       <c r="G64" s="17"/>
       <c r="H64" s="18"/>
@@ -3601,11 +3603,11 @@
       <c r="A65" s="14"/>
       <c r="B65" s="15"/>
       <c r="C65" s="15"/>
-      <c r="D65" s="41" t="str">
+      <c r="D65" s="41"/>
+      <c r="E65" s="43" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="E65" s="16"/>
       <c r="F65" s="16"/>
       <c r="G65" s="17"/>
       <c r="H65" s="18"/>
@@ -3621,11 +3623,11 @@
       <c r="A66" s="14"/>
       <c r="B66" s="15"/>
       <c r="C66" s="15"/>
-      <c r="D66" s="41" t="str">
+      <c r="D66" s="41"/>
+      <c r="E66" s="43" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="E66" s="16"/>
       <c r="F66" s="16"/>
       <c r="G66" s="17"/>
       <c r="H66" s="18"/>
@@ -3641,11 +3643,11 @@
       <c r="A67" s="14"/>
       <c r="B67" s="15"/>
       <c r="C67" s="15"/>
-      <c r="D67" s="41" t="str">
+      <c r="D67" s="41"/>
+      <c r="E67" s="43" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="E67" s="16"/>
       <c r="F67" s="16"/>
       <c r="G67" s="17"/>
       <c r="H67" s="18"/>
@@ -3661,11 +3663,11 @@
       <c r="A68" s="14"/>
       <c r="B68" s="15"/>
       <c r="C68" s="15"/>
-      <c r="D68" s="41" t="str">
+      <c r="D68" s="41"/>
+      <c r="E68" s="43" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="E68" s="16"/>
       <c r="F68" s="16"/>
       <c r="G68" s="17"/>
       <c r="H68" s="18"/>
@@ -3681,11 +3683,11 @@
       <c r="A69" s="14"/>
       <c r="B69" s="15"/>
       <c r="C69" s="15"/>
-      <c r="D69" s="41" t="str">
+      <c r="D69" s="41"/>
+      <c r="E69" s="43" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="E69" s="16"/>
       <c r="F69" s="16"/>
       <c r="G69" s="17"/>
       <c r="H69" s="18"/>
@@ -3701,11 +3703,11 @@
       <c r="A70" s="14"/>
       <c r="B70" s="15"/>
       <c r="C70" s="15"/>
-      <c r="D70" s="41" t="str">
+      <c r="D70" s="41"/>
+      <c r="E70" s="43" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="E70" s="16"/>
       <c r="F70" s="16"/>
       <c r="G70" s="17"/>
       <c r="H70" s="18"/>
@@ -3721,11 +3723,11 @@
       <c r="A71" s="14"/>
       <c r="B71" s="15"/>
       <c r="C71" s="15"/>
-      <c r="D71" s="41" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E71" s="16"/>
+      <c r="D71" s="41"/>
+      <c r="E71" s="43" t="str">
+        <f t="shared" ref="E71:E100" si="1">IF(AND(E$2="Yes",NOT(ISBLANK($C71))),C71,"")</f>
+        <v/>
+      </c>
       <c r="F71" s="16"/>
       <c r="G71" s="17"/>
       <c r="H71" s="18"/>
@@ -3741,11 +3743,11 @@
       <c r="A72" s="14"/>
       <c r="B72" s="15"/>
       <c r="C72" s="15"/>
-      <c r="D72" s="41" t="str">
-        <f t="shared" ref="D72:D100" si="1">IF(AND(E$2="Yes",NOT(ISBLANK($C72))),C72,"")</f>
-        <v/>
-      </c>
-      <c r="E72" s="16"/>
+      <c r="D72" s="41"/>
+      <c r="E72" s="43" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
       <c r="F72" s="16"/>
       <c r="G72" s="17"/>
       <c r="H72" s="18"/>
@@ -3761,11 +3763,11 @@
       <c r="A73" s="14"/>
       <c r="B73" s="15"/>
       <c r="C73" s="15"/>
-      <c r="D73" s="41" t="str">
+      <c r="D73" s="41"/>
+      <c r="E73" s="43" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="E73" s="16"/>
       <c r="F73" s="16"/>
       <c r="G73" s="17"/>
       <c r="H73" s="18"/>
@@ -3781,11 +3783,11 @@
       <c r="A74" s="14"/>
       <c r="B74" s="15"/>
       <c r="C74" s="15"/>
-      <c r="D74" s="41" t="str">
+      <c r="D74" s="41"/>
+      <c r="E74" s="43" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="E74" s="16"/>
       <c r="F74" s="16"/>
       <c r="G74" s="17"/>
       <c r="H74" s="18"/>
@@ -3801,11 +3803,11 @@
       <c r="A75" s="14"/>
       <c r="B75" s="15"/>
       <c r="C75" s="15"/>
-      <c r="D75" s="41" t="str">
+      <c r="D75" s="41"/>
+      <c r="E75" s="43" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="E75" s="16"/>
       <c r="F75" s="16"/>
       <c r="G75" s="17"/>
       <c r="H75" s="18"/>
@@ -3821,11 +3823,11 @@
       <c r="A76" s="14"/>
       <c r="B76" s="15"/>
       <c r="C76" s="15"/>
-      <c r="D76" s="41" t="str">
+      <c r="D76" s="41"/>
+      <c r="E76" s="43" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="E76" s="16"/>
       <c r="F76" s="16"/>
       <c r="G76" s="17"/>
       <c r="H76" s="18"/>
@@ -3841,11 +3843,11 @@
       <c r="A77" s="14"/>
       <c r="B77" s="15"/>
       <c r="C77" s="15"/>
-      <c r="D77" s="41" t="str">
+      <c r="D77" s="41"/>
+      <c r="E77" s="43" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="E77" s="16"/>
       <c r="F77" s="16"/>
       <c r="G77" s="17"/>
       <c r="H77" s="18"/>
@@ -3861,11 +3863,11 @@
       <c r="A78" s="14"/>
       <c r="B78" s="15"/>
       <c r="C78" s="15"/>
-      <c r="D78" s="41" t="str">
+      <c r="D78" s="41"/>
+      <c r="E78" s="43" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="E78" s="16"/>
       <c r="F78" s="16"/>
       <c r="G78" s="17"/>
       <c r="H78" s="18"/>
@@ -3881,11 +3883,11 @@
       <c r="A79" s="14"/>
       <c r="B79" s="15"/>
       <c r="C79" s="15"/>
-      <c r="D79" s="41" t="str">
+      <c r="D79" s="41"/>
+      <c r="E79" s="43" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="E79" s="16"/>
       <c r="F79" s="16"/>
       <c r="G79" s="17"/>
       <c r="H79" s="18"/>
@@ -3901,11 +3903,11 @@
       <c r="A80" s="14"/>
       <c r="B80" s="15"/>
       <c r="C80" s="15"/>
-      <c r="D80" s="41" t="str">
+      <c r="D80" s="41"/>
+      <c r="E80" s="43" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="E80" s="16"/>
       <c r="F80" s="16"/>
       <c r="G80" s="17"/>
       <c r="H80" s="18"/>
@@ -3921,11 +3923,11 @@
       <c r="A81" s="14"/>
       <c r="B81" s="15"/>
       <c r="C81" s="15"/>
-      <c r="D81" s="41" t="str">
+      <c r="D81" s="41"/>
+      <c r="E81" s="43" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="E81" s="16"/>
       <c r="F81" s="16"/>
       <c r="G81" s="17"/>
       <c r="H81" s="18"/>
@@ -3941,11 +3943,11 @@
       <c r="A82" s="14"/>
       <c r="B82" s="15"/>
       <c r="C82" s="15"/>
-      <c r="D82" s="41" t="str">
+      <c r="D82" s="41"/>
+      <c r="E82" s="43" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="E82" s="16"/>
       <c r="F82" s="16"/>
       <c r="G82" s="17"/>
       <c r="H82" s="18"/>
@@ -3961,11 +3963,11 @@
       <c r="A83" s="14"/>
       <c r="B83" s="15"/>
       <c r="C83" s="15"/>
-      <c r="D83" s="41" t="str">
+      <c r="D83" s="41"/>
+      <c r="E83" s="43" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="E83" s="16"/>
       <c r="F83" s="16"/>
       <c r="G83" s="17"/>
       <c r="H83" s="18"/>
@@ -3981,11 +3983,11 @@
       <c r="A84" s="14"/>
       <c r="B84" s="15"/>
       <c r="C84" s="15"/>
-      <c r="D84" s="41" t="str">
+      <c r="D84" s="41"/>
+      <c r="E84" s="43" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="E84" s="16"/>
       <c r="F84" s="16"/>
       <c r="G84" s="17"/>
       <c r="H84" s="18"/>
@@ -4001,11 +4003,11 @@
       <c r="A85" s="14"/>
       <c r="B85" s="15"/>
       <c r="C85" s="15"/>
-      <c r="D85" s="41" t="str">
+      <c r="D85" s="41"/>
+      <c r="E85" s="43" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="E85" s="16"/>
       <c r="F85" s="16"/>
       <c r="G85" s="17"/>
       <c r="H85" s="18"/>
@@ -4021,11 +4023,11 @@
       <c r="A86" s="14"/>
       <c r="B86" s="15"/>
       <c r="C86" s="15"/>
-      <c r="D86" s="41" t="str">
+      <c r="D86" s="41"/>
+      <c r="E86" s="43" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="E86" s="16"/>
       <c r="F86" s="16"/>
       <c r="G86" s="17"/>
       <c r="H86" s="18"/>
@@ -4041,11 +4043,11 @@
       <c r="A87" s="14"/>
       <c r="B87" s="15"/>
       <c r="C87" s="15"/>
-      <c r="D87" s="41" t="str">
+      <c r="D87" s="41"/>
+      <c r="E87" s="43" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="E87" s="16"/>
       <c r="F87" s="16"/>
       <c r="G87" s="17"/>
       <c r="H87" s="18"/>
@@ -4061,11 +4063,11 @@
       <c r="A88" s="14"/>
       <c r="B88" s="15"/>
       <c r="C88" s="15"/>
-      <c r="D88" s="41" t="str">
+      <c r="D88" s="41"/>
+      <c r="E88" s="43" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="E88" s="16"/>
       <c r="F88" s="16"/>
       <c r="G88" s="17"/>
       <c r="H88" s="18"/>
@@ -4081,11 +4083,11 @@
       <c r="A89" s="14"/>
       <c r="B89" s="15"/>
       <c r="C89" s="15"/>
-      <c r="D89" s="41" t="str">
+      <c r="D89" s="41"/>
+      <c r="E89" s="43" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="E89" s="16"/>
       <c r="F89" s="16"/>
       <c r="G89" s="17"/>
       <c r="H89" s="18"/>
@@ -4101,11 +4103,11 @@
       <c r="A90" s="14"/>
       <c r="B90" s="15"/>
       <c r="C90" s="15"/>
-      <c r="D90" s="41" t="str">
+      <c r="D90" s="41"/>
+      <c r="E90" s="43" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="E90" s="16"/>
       <c r="F90" s="16"/>
       <c r="G90" s="17"/>
       <c r="H90" s="18"/>
@@ -4121,11 +4123,11 @@
       <c r="A91" s="14"/>
       <c r="B91" s="15"/>
       <c r="C91" s="15"/>
-      <c r="D91" s="41" t="str">
+      <c r="D91" s="41"/>
+      <c r="E91" s="43" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="E91" s="16"/>
       <c r="F91" s="16"/>
       <c r="G91" s="17"/>
       <c r="H91" s="18"/>
@@ -4141,11 +4143,11 @@
       <c r="A92" s="14"/>
       <c r="B92" s="15"/>
       <c r="C92" s="15"/>
-      <c r="D92" s="41" t="str">
+      <c r="D92" s="41"/>
+      <c r="E92" s="43" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="E92" s="16"/>
       <c r="F92" s="16"/>
       <c r="G92" s="17"/>
       <c r="H92" s="18"/>
@@ -4161,11 +4163,11 @@
       <c r="A93" s="14"/>
       <c r="B93" s="15"/>
       <c r="C93" s="15"/>
-      <c r="D93" s="41" t="str">
+      <c r="D93" s="41"/>
+      <c r="E93" s="43" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="E93" s="16"/>
       <c r="F93" s="16"/>
       <c r="G93" s="17"/>
       <c r="H93" s="18"/>
@@ -4181,11 +4183,11 @@
       <c r="A94" s="14"/>
       <c r="B94" s="15"/>
       <c r="C94" s="15"/>
-      <c r="D94" s="41" t="str">
+      <c r="D94" s="41"/>
+      <c r="E94" s="43" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="E94" s="16"/>
       <c r="F94" s="16"/>
       <c r="G94" s="17"/>
       <c r="H94" s="18"/>
@@ -4201,11 +4203,11 @@
       <c r="A95" s="14"/>
       <c r="B95" s="15"/>
       <c r="C95" s="15"/>
-      <c r="D95" s="41" t="str">
+      <c r="D95" s="41"/>
+      <c r="E95" s="43" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="E95" s="16"/>
       <c r="F95" s="16"/>
       <c r="G95" s="17"/>
       <c r="H95" s="18"/>
@@ -4221,11 +4223,11 @@
       <c r="A96" s="14"/>
       <c r="B96" s="15"/>
       <c r="C96" s="15"/>
-      <c r="D96" s="41" t="str">
+      <c r="D96" s="41"/>
+      <c r="E96" s="43" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="E96" s="16"/>
       <c r="F96" s="16"/>
       <c r="G96" s="17"/>
       <c r="H96" s="18"/>
@@ -4241,11 +4243,11 @@
       <c r="A97" s="14"/>
       <c r="B97" s="15"/>
       <c r="C97" s="15"/>
-      <c r="D97" s="41" t="str">
+      <c r="D97" s="41"/>
+      <c r="E97" s="43" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="E97" s="16"/>
       <c r="F97" s="16"/>
       <c r="G97" s="17"/>
       <c r="H97" s="18"/>
@@ -4261,11 +4263,11 @@
       <c r="A98" s="14"/>
       <c r="B98" s="15"/>
       <c r="C98" s="15"/>
-      <c r="D98" s="41" t="str">
+      <c r="D98" s="41"/>
+      <c r="E98" s="43" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="E98" s="16"/>
       <c r="F98" s="16"/>
       <c r="G98" s="17"/>
       <c r="H98" s="18"/>
@@ -4281,11 +4283,11 @@
       <c r="A99" s="14"/>
       <c r="B99" s="15"/>
       <c r="C99" s="15"/>
-      <c r="D99" s="41" t="str">
+      <c r="D99" s="41"/>
+      <c r="E99" s="43" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="E99" s="16"/>
       <c r="F99" s="16"/>
       <c r="G99" s="17"/>
       <c r="H99" s="18"/>
@@ -4301,11 +4303,11 @@
       <c r="A100" s="14"/>
       <c r="B100" s="15"/>
       <c r="C100" s="15"/>
-      <c r="D100" s="41" t="str">
+      <c r="D100" s="41"/>
+      <c r="E100" s="43" t="str">
         <f>IF(AND(E$2="Yes",NOT(ISBLANK($C100))),C100,"")</f>
         <v/>
       </c>
-      <c r="E100" s="16"/>
       <c r="F100" s="16"/>
       <c r="G100" s="17"/>
       <c r="H100" s="18"/>
@@ -4321,11 +4323,11 @@
       <c r="A101" s="24"/>
       <c r="B101" s="25"/>
       <c r="C101" s="25"/>
-      <c r="D101" s="42" t="str">
+      <c r="D101" s="42"/>
+      <c r="E101" s="44" t="str">
         <f>IF(AND(E$2="Yes",NOT(ISBLANK($C101))),C101,"")</f>
         <v/>
       </c>
-      <c r="E101" s="26"/>
       <c r="F101" s="26"/>
       <c r="G101" s="27"/>
       <c r="H101" s="28"/>
@@ -4945,11 +4947,12 @@
     <row r="707" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="708" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J6:J101" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"YES,NO"</formula1>
       <formula2>0</formula2>
     </dataValidation>
+    <dataValidation allowBlank="1" showErrorMessage="1" sqref="E101 E6:E99 E100" xr:uid="{62359B35-AF9C-184B-BA2B-D61024C8A4D0}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
@@ -4963,7 +4966,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>C6:C101 E6:E101 I6:I101</xm:sqref>
+          <xm:sqref>C6:C101 I6:I101</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
           <x14:formula1>
@@ -5008,7 +5011,7 @@
   <sheetData>
     <row r="1" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -5058,7 +5061,7 @@
     </row>
     <row r="3" spans="1:22" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -5108,7 +5111,7 @@
     </row>
     <row r="5" spans="1:22" ht="21" x14ac:dyDescent="0.25">
       <c r="A5" s="34" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
@@ -5154,10 +5157,10 @@
     </row>
     <row r="7" spans="1:22" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="36" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7" s="37" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C7" s="38"/>
       <c r="D7" s="3"/>
@@ -5182,10 +5185,10 @@
     </row>
     <row r="8" spans="1:22" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="36" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" s="37" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C8" s="38"/>
       <c r="D8" s="3"/>
@@ -5210,10 +5213,10 @@
     </row>
     <row r="9" spans="1:22" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="36" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C9" s="38"/>
       <c r="D9" s="3"/>
@@ -5238,10 +5241,10 @@
     </row>
     <row r="10" spans="1:22" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="36" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" s="37" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C10" s="38"/>
       <c r="D10" s="3"/>
@@ -5266,10 +5269,10 @@
     </row>
     <row r="11" spans="1:22" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="36" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" s="37" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C11" s="38"/>
       <c r="D11" s="3"/>
@@ -5294,10 +5297,10 @@
     </row>
     <row r="12" spans="1:22" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="36" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12" s="37" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C12" s="38"/>
       <c r="D12" s="3"/>
@@ -5322,10 +5325,10 @@
     </row>
     <row r="13" spans="1:22" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="36" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B13" s="37" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C13" s="38"/>
       <c r="D13" s="3"/>
@@ -5350,10 +5353,10 @@
     </row>
     <row r="14" spans="1:22" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="36" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B14" s="37" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C14" s="38"/>
       <c r="D14" s="3"/>
@@ -5378,10 +5381,10 @@
     </row>
     <row r="15" spans="1:22" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="36" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B15" s="37" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C15" s="38"/>
       <c r="D15" s="3"/>
@@ -5406,10 +5409,10 @@
     </row>
     <row r="16" spans="1:22" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="36" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B16" s="37" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C16" s="38"/>
       <c r="D16" s="3"/>
@@ -5434,10 +5437,10 @@
     </row>
     <row r="17" spans="1:22" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="36" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B17" s="37" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C17" s="38"/>
       <c r="D17" s="3"/>
@@ -5462,10 +5465,10 @@
     </row>
     <row r="18" spans="1:22" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="36" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B18" s="37" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C18" s="38"/>
       <c r="D18" s="3"/>
@@ -5490,10 +5493,10 @@
     </row>
     <row r="19" spans="1:22" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="36" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B19" s="37" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C19" s="38"/>
       <c r="D19" s="3"/>
@@ -5518,10 +5521,10 @@
     </row>
     <row r="20" spans="1:22" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="36" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B20" s="37" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C20" s="38"/>
       <c r="D20" s="3"/>
@@ -5546,10 +5549,10 @@
     </row>
     <row r="21" spans="1:22" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="36" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B21" s="37" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C21" s="38"/>
       <c r="D21" s="3"/>
@@ -6211,2275 +6214,2275 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>39</v>
-      </c>
       <c r="D1" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E1" s="39" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>42</v>
-      </c>
       <c r="E2" s="39" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>45</v>
-      </c>
       <c r="E3" s="39" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>49</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>53</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>61</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C12" s="3"/>
     </row>
     <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C13" s="3"/>
     </row>
     <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>65</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>66</v>
       </c>
       <c r="C14" s="3"/>
     </row>
     <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>67</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>69</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>71</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>73</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>75</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>77</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>79</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>81</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>83</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>85</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B25" s="3" t="s">
         <v>87</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B38" s="3" t="s">
         <v>101</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B39" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B40" s="3" t="s">
         <v>105</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B41" s="3" t="s">
         <v>107</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B42" s="3" t="s">
         <v>109</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B43" s="3" t="s">
         <v>111</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B44" s="3" t="s">
         <v>113</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B45" s="3" t="s">
         <v>115</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B46" s="3" t="s">
         <v>117</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B47" s="3" t="s">
         <v>119</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B48" s="3" t="s">
         <v>121</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B49" s="3" t="s">
         <v>123</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B62" s="3" t="s">
         <v>137</v>
-      </c>
-      <c r="B62" s="3" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B63" s="3" t="s">
         <v>139</v>
-      </c>
-      <c r="B63" s="3" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B64" s="3" t="s">
         <v>141</v>
-      </c>
-      <c r="B64" s="3" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B65" s="3" t="s">
         <v>143</v>
-      </c>
-      <c r="B65" s="3" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B66" s="3" t="s">
         <v>145</v>
-      </c>
-      <c r="B66" s="3" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B67" s="3" t="s">
         <v>147</v>
-      </c>
-      <c r="B67" s="3" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B68" s="3" t="s">
         <v>149</v>
-      </c>
-      <c r="B68" s="3" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B69" s="3" t="s">
         <v>151</v>
-      </c>
-      <c r="B69" s="3" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B70" s="3" t="s">
         <v>153</v>
-      </c>
-      <c r="B70" s="3" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B71" s="3" t="s">
         <v>155</v>
-      </c>
-      <c r="B71" s="3" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B72" s="3" t="s">
         <v>157</v>
-      </c>
-      <c r="B72" s="3" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B73" s="3" t="s">
         <v>159</v>
-      </c>
-      <c r="B73" s="3" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="B86" s="3" t="s">
         <v>173</v>
-      </c>
-      <c r="B86" s="3" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="B87" s="3" t="s">
         <v>175</v>
-      </c>
-      <c r="B87" s="3" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="B88" s="3" t="s">
         <v>177</v>
-      </c>
-      <c r="B88" s="3" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B89" s="3" t="s">
         <v>179</v>
-      </c>
-      <c r="B89" s="3" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="B90" s="3" t="s">
         <v>181</v>
-      </c>
-      <c r="B90" s="3" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="B91" s="3" t="s">
         <v>183</v>
-      </c>
-      <c r="B91" s="3" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="B92" s="3" t="s">
         <v>185</v>
-      </c>
-      <c r="B92" s="3" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="B93" s="3" t="s">
         <v>187</v>
-      </c>
-      <c r="B93" s="3" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="B94" s="3" t="s">
         <v>189</v>
-      </c>
-      <c r="B94" s="3" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="B95" s="3" t="s">
         <v>191</v>
-      </c>
-      <c r="B95" s="3" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="B96" s="3" t="s">
         <v>193</v>
-      </c>
-      <c r="B96" s="3" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="B97" s="3" t="s">
         <v>195</v>
-      </c>
-      <c r="B97" s="3" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B98" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B99" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B100" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B101" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B102" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B103" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B104" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B105" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B106" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B107" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B108" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B109" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B110" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B111" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B112" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="113" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B113" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="114" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B114" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="115" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B115" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="116" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B116" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="117" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B117" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="118" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B118" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="119" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B119" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="120" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B120" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="121" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B121" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="122" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B122" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="123" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B123" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="124" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B124" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="125" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B125" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="126" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B126" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="127" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B127" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="128" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B128" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="129" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B129" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="130" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B130" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="131" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B131" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="132" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B132" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="133" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B133" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="134" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B134" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="135" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B135" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="136" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B136" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="137" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B137" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="138" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B138" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="139" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B139" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="140" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B140" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="141" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B141" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="142" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B142" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="143" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B143" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="144" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B144" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="145" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B145" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="146" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B146" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="147" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B147" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="148" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B148" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="149" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B149" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="150" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B150" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="151" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B151" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="152" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B152" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="153" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B153" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="154" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B154" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="155" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B155" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="156" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B156" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="157" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B157" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="158" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B158" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="159" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B159" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="160" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B160" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="161" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B161" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="162" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B162" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="163" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B163" s="3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="164" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B164" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="165" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B165" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="166" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B166" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="167" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B167" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="168" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B168" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="169" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B169" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="170" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B170" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="171" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B171" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="172" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B172" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="173" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B173" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="174" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B174" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="175" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B175" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="176" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B176" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="177" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B177" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="178" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B178" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="179" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B179" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="180" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B180" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="181" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B181" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="182" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B182" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="183" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B183" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="184" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B184" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="185" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B185" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="186" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B186" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="187" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B187" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="188" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B188" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="189" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B189" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="190" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B190" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="191" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B191" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="192" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B192" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="193" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B193" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="194" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B194" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="195" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B195" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="196" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B196" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="197" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B197" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="198" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B198" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="199" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B199" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="200" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B200" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="201" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B201" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="202" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B202" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="203" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B203" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="204" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B204" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="205" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B205" s="3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="206" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B206" s="3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="207" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B207" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="208" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B208" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="209" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B209" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="210" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B210" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="211" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B211" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="212" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B212" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="213" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B213" s="3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="214" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B214" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="215" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B215" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="216" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B216" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="217" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B217" s="3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="218" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B218" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="219" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B219" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="220" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B220" s="3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="221" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B221" s="3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="222" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B222" s="3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="223" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B223" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="224" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B224" s="3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="225" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B225" s="3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="226" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B226" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="227" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B227" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="228" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B228" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="229" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B229" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="230" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B230" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="231" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B231" s="3" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="232" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B232" s="3" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="233" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B233" s="3" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="234" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B234" s="3" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="235" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B235" s="3" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="236" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B236" s="3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="237" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B237" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="238" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B238" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="239" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B239" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="240" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B240" s="3" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="241" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B241" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="242" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B242" s="3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="243" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B243" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="244" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B244" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="245" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B245" s="3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="246" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B246" s="3" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="247" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B247" s="3" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="248" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B248" s="3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="249" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B249" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="250" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B250" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="251" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B251" s="3" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="252" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B252" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="253" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B253" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="254" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B254" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="255" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B255" s="3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="256" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B256" s="3" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="257" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B257" s="3" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="258" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B258" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="259" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B259" s="3" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="260" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B260" s="3" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="261" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B261" s="3" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="262" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B262" s="3" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="263" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B263" s="3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="264" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B264" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="265" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B265" s="3" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="266" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B266" s="3" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="267" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B267" s="3" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="268" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B268" s="3" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="269" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B269" s="3" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="270" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B270" s="3" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="271" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B271" s="3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="272" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B272" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="273" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B273" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="274" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B274" s="3" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="275" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B275" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="276" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B276" s="3" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="277" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B277" s="3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="278" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B278" s="3" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="279" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B279" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="280" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B280" s="3" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="281" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B281" s="3" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="282" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B282" s="3" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="283" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B283" s="3" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="284" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B284" s="3" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="285" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B285" s="3" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="286" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B286" s="3" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="287" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B287" s="3" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="288" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B288" s="3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="289" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B289" s="3" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="290" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B290" s="3" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="291" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B291" s="3" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="292" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B292" s="3" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="293" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B293" s="3" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="294" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B294" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="295" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B295" s="3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="296" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B296" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="297" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B297" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="298" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B298" s="3" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="299" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B299" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="300" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B300" s="3" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="301" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B301" s="3" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="302" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B302" s="3" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="303" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B303" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="304" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B304" s="3" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="305" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B305" s="3" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="306" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B306" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="307" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B307" s="3" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="308" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B308" s="3" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="309" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B309" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="310" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B310" s="3" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="311" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B311" s="3" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="312" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B312" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="313" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B313" s="3" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="314" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B314" s="3" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="315" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B315" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="316" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B316" s="3" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="317" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B317" s="3" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="318" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B318" s="3" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="319" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B319" s="3" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="320" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B320" s="3" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="321" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B321" s="3" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="322" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B322" s="3" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="323" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B323" s="3" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="324" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B324" s="3" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="325" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B325" s="3" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="326" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B326" s="3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="327" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B327" s="3" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="328" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B328" s="3" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="329" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B329" s="3" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="330" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B330" s="3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="331" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B331" s="3" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="332" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B332" s="3" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="333" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B333" s="3" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="334" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B334" s="3" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="335" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B335" s="3" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="336" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B336" s="3" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="337" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B337" s="3" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="338" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B338" s="3" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="339" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B339" s="3" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="340" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B340" s="3" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="341" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B341" s="3" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="342" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B342" s="3" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="343" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B343" s="3" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="344" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B344" s="3" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="345" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B345" s="3" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="346" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B346" s="3" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="347" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B347" s="3" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="348" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B348" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="349" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B349" s="3" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="350" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B350" s="3" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="351" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B351" s="3" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="352" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B352" s="3" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="353" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B353" s="3" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="354" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B354" s="3" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="355" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B355" s="3" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="356" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B356" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="357" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B357" s="3" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="358" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B358" s="3" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="359" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B359" s="3" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="360" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B360" s="3" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="361" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B361" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="362" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B362" s="3" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="363" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B363" s="3" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="364" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B364" s="3" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="365" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B365" s="3" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="366" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B366" s="3" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="367" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B367" s="3" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="368" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B368" s="3" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="369" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B369" s="3" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="370" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B370" s="3" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="371" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B371" s="3" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="372" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B372" s="3" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="373" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B373" s="3" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="374" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B374" s="3" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="375" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B375" s="3" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="376" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B376" s="3" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="377" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B377" s="3" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="378" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B378" s="3" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="379" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B379" s="3" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="380" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B380" s="3" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="381" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B381" s="3" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="382" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B382" s="3" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="383" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B383" s="3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="384" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B384" s="3" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="385" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B385" s="3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="386" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
adding destination coords to info sheet
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Sample_transfer_v4_6_0.xlsx
+++ b/backend/fms_core/static/submission_templates/Sample_transfer_v4_6_0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jmarcelino/Desktop/freezeman/backend/fms_core/static/submission_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D78A9468-2F54-1D46-A509-35ACF35AE69A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65F76420-B8C0-DE48-9E0F-3B6FC805A1BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="8080" windowWidth="27040" windowHeight="11560" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="6000" windowWidth="27040" windowHeight="11560" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SampleTransfer" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="439">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="440">
   <si>
     <t>Sample Transfer Template</t>
   </si>
@@ -1383,6 +1383,9 @@
   </si>
   <si>
     <t>Version : 4.6.0</t>
+  </si>
+  <si>
+    <t>If the "Destination Container Coord" is set to "Yes" the destination coordinates will be set to the source coordinates.</t>
   </si>
 </sst>
 </file>
@@ -1496,7 +1499,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -1838,11 +1841,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1914,8 +1926,9 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2300,7 +2313,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD708"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
@@ -3725,7 +3738,7 @@
       <c r="C71" s="15"/>
       <c r="D71" s="41"/>
       <c r="E71" s="43" t="str">
-        <f t="shared" ref="E71:E100" si="1">IF(AND(E$2="Yes",NOT(ISBLANK($C71))),C71,"")</f>
+        <f t="shared" ref="E71:E99" si="1">IF(AND(E$2="Yes",NOT(ISBLANK($C71))),C71,"")</f>
         <v/>
       </c>
       <c r="F71" s="16"/>
@@ -5000,9 +5013,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:V54"/>
+  <dimension ref="A1:V55"/>
   <sheetViews>
-    <sheetView zoomScale="91" zoomScaleNormal="91" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
@@ -5086,7 +5101,9 @@
       <c r="V3" s="3"/>
     </row>
     <row r="4" spans="1:22" ht="15" x14ac:dyDescent="0.2">
-      <c r="A4" s="3"/>
+      <c r="A4" s="3" t="s">
+        <v>439</v>
+      </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -5109,10 +5126,9 @@
       <c r="U4" s="3"/>
       <c r="V4" s="3"/>
     </row>
-    <row r="5" spans="1:22" ht="21" x14ac:dyDescent="0.25">
-      <c r="A5" s="34" t="s">
-        <v>20</v>
-      </c>
+    <row r="5" spans="1:22" ht="15" x14ac:dyDescent="0.2">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
@@ -5133,8 +5149,10 @@
       <c r="U5" s="3"/>
       <c r="V5" s="3"/>
     </row>
-    <row r="6" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="B6" s="35"/>
+    <row r="6" spans="1:22" ht="21" x14ac:dyDescent="0.25">
+      <c r="A6" s="34" t="s">
+        <v>20</v>
+      </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
@@ -5156,13 +5174,8 @@
       <c r="V6" s="3"/>
     </row>
     <row r="7" spans="1:22" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="36" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="37" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="38"/>
+      <c r="B7" s="35"/>
+      <c r="C7" s="45"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
@@ -5185,12 +5198,12 @@
     </row>
     <row r="8" spans="1:22" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="36" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B8" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="38"/>
+        <v>21</v>
+      </c>
+      <c r="C8" s="45"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
@@ -5213,10 +5226,10 @@
     </row>
     <row r="9" spans="1:22" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="36" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C9" s="38"/>
       <c r="D9" s="3"/>
@@ -5241,10 +5254,10 @@
     </row>
     <row r="10" spans="1:22" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="36" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B10" s="37" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C10" s="38"/>
       <c r="D10" s="3"/>
@@ -5269,10 +5282,10 @@
     </row>
     <row r="11" spans="1:22" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="36" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B11" s="37" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C11" s="38"/>
       <c r="D11" s="3"/>
@@ -5297,10 +5310,10 @@
     </row>
     <row r="12" spans="1:22" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="36" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B12" s="37" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C12" s="38"/>
       <c r="D12" s="3"/>
@@ -5325,10 +5338,10 @@
     </row>
     <row r="13" spans="1:22" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="36" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B13" s="37" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C13" s="38"/>
       <c r="D13" s="3"/>
@@ -5353,10 +5366,10 @@
     </row>
     <row r="14" spans="1:22" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="36" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B14" s="37" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C14" s="38"/>
       <c r="D14" s="3"/>
@@ -5381,10 +5394,10 @@
     </row>
     <row r="15" spans="1:22" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="36" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B15" s="37" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C15" s="38"/>
       <c r="D15" s="3"/>
@@ -5409,10 +5422,10 @@
     </row>
     <row r="16" spans="1:22" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="36" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B16" s="37" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C16" s="38"/>
       <c r="D16" s="3"/>
@@ -5437,10 +5450,10 @@
     </row>
     <row r="17" spans="1:22" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="36" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B17" s="37" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C17" s="38"/>
       <c r="D17" s="3"/>
@@ -5465,10 +5478,10 @@
     </row>
     <row r="18" spans="1:22" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="36" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B18" s="37" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C18" s="38"/>
       <c r="D18" s="3"/>
@@ -5493,10 +5506,10 @@
     </row>
     <row r="19" spans="1:22" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="36" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B19" s="37" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C19" s="38"/>
       <c r="D19" s="3"/>
@@ -5521,10 +5534,10 @@
     </row>
     <row r="20" spans="1:22" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="36" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B20" s="37" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C20" s="38"/>
       <c r="D20" s="3"/>
@@ -5549,10 +5562,10 @@
     </row>
     <row r="21" spans="1:22" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="36" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B21" s="37" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C21" s="38"/>
       <c r="D21" s="3"/>
@@ -5575,9 +5588,13 @@
       <c r="U21" s="3"/>
       <c r="V21" s="3"/>
     </row>
-    <row r="22" spans="1:22" ht="15" x14ac:dyDescent="0.2">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
+    <row r="22" spans="1:22" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" s="37" t="s">
+        <v>35</v>
+      </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
@@ -5600,6 +5617,8 @@
       <c r="V22" s="3"/>
     </row>
     <row r="23" spans="1:22" ht="15" x14ac:dyDescent="0.2">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
       <c r="N23" s="3"/>
       <c r="O23" s="3"/>
       <c r="P23" s="3"/>
@@ -5754,8 +5773,6 @@
       <c r="V36" s="3"/>
     </row>
     <row r="37" spans="1:22" ht="15" x14ac:dyDescent="0.2">
-      <c r="A37" s="3"/>
-      <c r="B37" s="3"/>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
@@ -6184,6 +6201,10 @@
       <c r="T54" s="3"/>
       <c r="U54" s="3"/>
       <c r="V54" s="3"/>
+    </row>
+    <row r="55" spans="1:22" ht="15" x14ac:dyDescent="0.2">
+      <c r="A55" s="3"/>
+      <c r="B55" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>

</xml_diff>

<commit_message>
fixing template on open
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Sample_transfer_v4_6_0.xlsx
+++ b/backend/fms_core/static/submission_templates/Sample_transfer_v4_6_0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jmarcelino/Desktop/freezeman/backend/fms_core/static/submission_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06996492-146A-DB47-83A2-A83D749551D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B831171C-20CD-7441-9338-8C865BFCF8BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="6000" windowWidth="27040" windowHeight="11560" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="320" yWindow="2200" windowWidth="27040" windowHeight="11560" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SampleTransfer" sheetId="1" r:id="rId1"/>
@@ -2316,9 +2316,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD708"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -6223,7 +6223,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>

</xml_diff>